<commit_message>
category excel upload done, category ddl integration try
</commit_message>
<xml_diff>
--- a/Scomm/wwwroot/Uploads/ItemExcel.xlsx
+++ b/Scomm/wwwroot/Uploads/ItemExcel.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zaber\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zaber-Desktop\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4187947-C370-4B3F-9EA9-72781F7E00A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,22 +363,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="2"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,7 +395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -407,10 +406,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
         <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>